<commit_message>
actualización de documentación y frontend
</commit_message>
<xml_diff>
--- a/Files/normalizaciones.xlsx
+++ b/Files/normalizaciones.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/milcavaldez/Documents/MarketApp/Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/milcavaldez/Documents/Marketfy/Marketfy/Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409973DE-184A-874A-B271-2BA633F87956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A34474D-4083-1644-830C-FFC5D4D99A41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20300" xr2:uid="{F89B3924-7BA0-224A-835B-B853078A7A53}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20160" xr2:uid="{F89B3924-7BA0-224A-835B-B853078A7A53}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -682,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC84F830-DD3A-8240-B228-CDC1C4B11B99}">
   <dimension ref="A3:K84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>